<commit_message>
updating to add battery preprocessing
</commit_message>
<xml_diff>
--- a/Stochastic_engine/scenario_parameters.xlsx
+++ b/Stochastic_engine/scenario_parameters.xlsx
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5420.730743926406</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>327.65</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>